<commit_message>
DP: create_forecast_basic future - change_pop_to_iplan_goals_till_2050_230711.ipynb - change global_functions location
</commit_message>
<xml_diff>
--- a/create_forecast_basic/future/bau/inputs_outputs.xlsx
+++ b/create_forecast_basic/future/bau/inputs_outputs.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t xml:space="preserve">discription</t>
   </si>
@@ -38,9 +38,6 @@
   </si>
   <si>
     <t xml:space="preserve">C:\Users\dpere\Documents\JTMT\forecast_by_version\V4\BASE_YEAR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">W:\Data\Forecast\forecast_by_version\V4\BASE_YEAR</t>
   </si>
 </sst>
 </file>
@@ -148,7 +145,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.37890625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -181,11 +178,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>